<commit_message>
Adding classes to start the annotation process with PathwayCommons
</commit_message>
<xml_diff>
--- a/TimeTests.xlsx
+++ b/TimeTests.xlsx
@@ -19,16 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>mdr.cv(data, K=2, cv=5, genotype=c(0,1,2))</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Samples</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>User Time</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -42,6 +38,22 @@
   </si>
   <si>
     <t>mdr.cv(data, K=4, cv=5, genotype=c(0,1,2))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Java Tool K=2 cv=5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SNPs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Java Tool K=4 cv=5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stopped after 20 min with no pg</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -49,12 +61,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -425,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -443,16 +449,16 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -537,7 +543,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -569,8 +575,33 @@
         <v>500</v>
       </c>
     </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>500</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2.7083333333333334E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>500</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>